<commit_message>
Added implementation for divide and conquer approach
</commit_message>
<xml_diff>
--- a/algorithms/adjmatrix.xlsx
+++ b/algorithms/adjmatrix.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sushrit/Documents/1.SIUE/Courses/Spring2024/Design of algorithms/Project/WebApp/DataSet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sushrit/Documents/1.SIUE/Courses/Spring2024/Design of algorithms/Project/WebApp/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44D2D993-F903-D148-93C0-045E1FC43C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56630F1E-A5A4-8745-B6E8-6617FA45B176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{F4ED4291-A30C-724C-8B57-2C7475F4AD32}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="33520" windowHeight="20500" xr2:uid="{F4ED4291-A30C-724C-8B57-2C7475F4AD32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,35 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
-  <si>
-    <t>EB</t>
-  </si>
-  <si>
-    <t>EF I</t>
-  </si>
-  <si>
-    <t>EF II</t>
-  </si>
-  <si>
-    <t>EF III</t>
-  </si>
-  <si>
-    <t>EPD</t>
-  </si>
-  <si>
-    <t>MPD</t>
-  </si>
-  <si>
-    <t>SPD</t>
-  </si>
-  <si>
-    <t>AH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EF II </t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,40 +389,47 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1">
+        <f>B1+1</f>
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1">
+        <f t="shared" ref="D1:I1" si="0">C1+1</f>
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="I1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -478,8 +457,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3.9</v>
@@ -507,8 +487,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
+      <c r="A4">
+        <f t="shared" ref="A4:A9" si="1">A3+1</f>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>4.3</v>
@@ -536,8 +517,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0.6</v>
@@ -565,8 +547,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -594,8 +577,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>4.4000000000000004</v>
@@ -623,8 +607,9 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1.7</v>
@@ -652,8 +637,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>5.5</v>

</xml_diff>